<commit_message>
info to case studies added
</commit_message>
<xml_diff>
--- a/src/components/survey_2.xlsx
+++ b/src/components/survey_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="caseStudies" sheetId="1" state="visible" r:id="rId2"/>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">Mailing address of the supervising organization</t>
   </si>
   <si>
-    <t xml:space="preserve">Conctacts</t>
+    <t xml:space="preserve">Contacts</t>
   </si>
   <si>
     <t xml:space="preserve">Wastewater treatment</t>
@@ -191,6 +191,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Life Remembrane:</t>
     </r>
@@ -199,6 +200,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> demonstration plant in which diverse mechanical and chemical treatments are developed in order to recover these membranes to reuse them in reverse osmosis technology </t>
     </r>
@@ -332,6 +334,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Eflucomp project:</t>
     </r>
@@ -340,6 +343,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Application of recycled membranes for treating industrial wastewater</t>
     </r>
@@ -349,6 +353,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -384,6 +389,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mem2.0: </t>
     </r>
@@ -392,6 +398,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Landfill leachate water treatment using end-of-life RO and regenerated membranes</t>
     </r>
@@ -454,6 +461,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">University of Girona (Spain) and University of New S</t>
     </r>
@@ -463,6 +471,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">outh Wales (Australia)</t>
     </r>
@@ -474,6 +483,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mem2.0:</t>
     </r>
@@ -482,6 +492,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Novel membrane housing designs for gravity-driven NF and UF recycled membrane-based systems</t>
     </r>
@@ -637,6 +648,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Life-Transfomem project. </t>
     </r>
@@ -645,6 +657,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Production of recycled UF membranes for seawater treatment as substitution of standard sand filtration</t>
     </r>
@@ -659,6 +672,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Life-Transfomem project. </t>
     </r>
@@ -667,6 +681,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Production of recycled UF membranes for wastewater treatment. Spiral-wound, semiopened and star configurations</t>
     </r>
@@ -712,6 +727,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Nextgenwater project:</t>
     </r>
@@ -721,6 +737,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Application of recyed UF membrane for water reclaiming</t>
     </r>
@@ -742,6 +759,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Regireu project</t>
     </r>
@@ -751,6 +769,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">: Application of recycled membranes for treating urban wastewater</t>
     </r>
@@ -892,6 +911,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Life-Releach:</t>
     </r>
@@ -900,6 +920,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> new landfill leachate treatment strategies based on the use of different existing technologies including recycled NF and RO membranes</t>
     </r>
@@ -945,6 +966,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mem2.0: </t>
     </r>
@@ -953,6 +975,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Novel membrane housing designs for gravity-driven NF and UF recycled membrane-based systems</t>
     </r>
@@ -972,6 +995,7 @@
         <sz val="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">INREMEM project: </t>
     </r>
@@ -981,6 +1005,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">innovation and recycling membranes  for water filtration(UF-MBR, FO, electrodyalisis, support)</t>
     </r>
@@ -1022,6 +1047,7 @@
         <sz val="10"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H2020 Remeb.</t>
     </r>
@@ -1031,6 +1057,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Implementation and validation of a low cost recycled ceramic membrane bioreactor (MBR) for water reuse in a Wastewater Treatment Plant (WWTP)</t>
     </r>
@@ -1129,6 +1156,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1150,6 +1178,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1157,23 +1186,27 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1181,6 +1214,7 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1188,18 +1222,21 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1207,12 +1244,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1220,12 +1259,14 @@
       <color rgb="FF3366FF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1324,13 +1365,15 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1415,14 +1458,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -1441,10 +1476,6 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1548,15 +1579,15 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="67.52"/>
@@ -2063,13 +2094,13 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="46.83"/>
@@ -2206,7 +2237,7 @@
       <c r="L3" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="15" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2247,7 +2278,7 @@
       <c r="L4" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="15" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2255,7 +2286,7 @@
       <c r="A5" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="17" t="s">
         <v>75</v>
       </c>
       <c r="C5" s="17" t="s">
@@ -2288,7 +2319,7 @@
       <c r="L5" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="15" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2329,7 +2360,7 @@
       <c r="L6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="15" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2361,7 +2392,7 @@
       <c r="I7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="21" t="s">
         <v>95</v>
       </c>
       <c r="K7" s="18" t="s">
@@ -2402,7 +2433,7 @@
       <c r="I8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="21" t="s">
         <v>104</v>
       </c>
       <c r="K8" s="18" t="s">
@@ -2419,7 +2450,7 @@
       <c r="A9" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="17" t="s">
         <v>108</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -2460,7 +2491,7 @@
       <c r="A10" s="15" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="17" t="s">
         <v>117</v>
       </c>
       <c r="C10" s="17" t="s">
@@ -2493,7 +2524,7 @@
       <c r="L10" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="22" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2504,7 +2535,7 @@
       <c r="B11" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>122</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -2525,7 +2556,7 @@
       <c r="I11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="21" t="s">
         <v>123</v>
       </c>
       <c r="K11" s="18" t="s">
@@ -2542,7 +2573,7 @@
       <c r="A12" s="15" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C12" s="17" t="s">
@@ -2583,7 +2614,7 @@
       <c r="A13" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -2624,7 +2655,7 @@
       <c r="A14" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -2665,7 +2696,7 @@
       <c r="A15" s="15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -2747,7 +2778,7 @@
       <c r="A17" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="17" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="17" t="s">
@@ -2788,7 +2819,7 @@
       <c r="A18" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="17" t="s">
         <v>166</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -2829,7 +2860,7 @@
       <c r="A19" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>169</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -2841,7 +2872,7 @@
       <c r="E19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="24" t="s">
         <v>171</v>
       </c>
       <c r="G19" s="19" t="s">
@@ -2856,7 +2887,7 @@
       <c r="J19" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="24" t="s">
         <v>173</v>
       </c>
       <c r="L19" s="17" t="s">
@@ -2870,7 +2901,7 @@
       <c r="A20" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -2882,7 +2913,7 @@
       <c r="E20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="24" t="s">
         <v>171</v>
       </c>
       <c r="G20" s="19" t="s">
@@ -2911,7 +2942,7 @@
       <c r="A21" s="15" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="17" t="s">
         <v>176</v>
       </c>
       <c r="C21" s="17" t="s">
@@ -2976,7 +3007,7 @@
       <c r="I22" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="25" t="s">
         <v>186</v>
       </c>
       <c r="K22" s="18" t="s">
@@ -3017,7 +3048,7 @@
       <c r="I23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="25" t="s">
         <v>190</v>
       </c>
       <c r="K23" s="18" t="s">
@@ -3034,7 +3065,7 @@
       <c r="A24" s="15" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="17" t="s">
         <v>192</v>
       </c>
       <c r="C24" s="17" t="s">
@@ -3108,7 +3139,7 @@
       <c r="L25" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="M25" s="21" t="s">
+      <c r="M25" s="15" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3157,7 +3188,7 @@
       <c r="A27" s="15" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="19" t="s">
         <v>215</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -3231,7 +3262,7 @@
       <c r="L28" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="M28" s="21" t="s">
+      <c r="M28" s="15" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3280,7 +3311,7 @@
       <c r="A30" s="15" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C30" s="17" t="s">
@@ -3324,7 +3355,7 @@
       <c r="B31" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="19" t="s">
         <v>177</v>
       </c>
       <c r="D31" s="19" t="s">
@@ -3383,10 +3414,10 @@
       <c r="H32" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="29" t="s">
+      <c r="I32" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="J32" s="30" t="s">
+      <c r="J32" s="27" t="s">
         <v>245</v>
       </c>
       <c r="K32" s="18" t="s">
@@ -3424,10 +3455,10 @@
       <c r="H33" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="29" t="s">
+      <c r="I33" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="J33" s="29" t="s">
+      <c r="J33" s="26" t="s">
         <v>249</v>
       </c>
       <c r="K33" s="18" t="s">
@@ -3465,10 +3496,10 @@
       <c r="H34" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="29" t="s">
+      <c r="I34" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="J34" s="29" t="s">
+      <c r="J34" s="26" t="s">
         <v>252</v>
       </c>
       <c r="K34" s="18" t="s">
@@ -3506,10 +3537,10 @@
       <c r="H35" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="29" t="s">
+      <c r="I35" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="J35" s="26" t="s">
         <v>254</v>
       </c>
       <c r="K35" s="18" t="s">
@@ -3547,10 +3578,10 @@
       <c r="H36" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="29" t="s">
+      <c r="I36" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="31" t="s">
+      <c r="J36" s="28" t="s">
         <v>260</v>
       </c>
       <c r="K36" s="18" t="s">
@@ -3559,7 +3590,7 @@
       <c r="L36" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="M36" s="32" t="s">
+      <c r="M36" s="29" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3588,10 +3619,10 @@
       <c r="H37" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="29" t="s">
+      <c r="I37" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="J37" s="29" t="s">
+      <c r="J37" s="26" t="s">
         <v>267</v>
       </c>
       <c r="K37" s="18" t="s">
@@ -3600,7 +3631,7 @@
       <c r="L37" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="M37" s="33" t="s">
+      <c r="M37" s="30" t="s">
         <v>270</v>
       </c>
     </row>
@@ -3629,10 +3660,10 @@
       <c r="H38" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="29" t="s">
+      <c r="I38" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="J38" s="29" t="s">
+      <c r="J38" s="26" t="s">
         <v>272</v>
       </c>
       <c r="K38" s="18" t="s">
@@ -3652,7 +3683,7 @@
       <c r="B39" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="C39" s="25" t="str">
+      <c r="C39" s="23" t="str">
         <f aca="false">D39</f>
         <v>Angers University, GEIHP</v>
       </c>
@@ -3671,10 +3702,10 @@
       <c r="H39" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="I39" s="29" t="s">
+      <c r="I39" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="J39" s="29" t="s">
+      <c r="J39" s="26" t="s">
         <v>278</v>
       </c>
       <c r="K39" s="18" t="s">
@@ -3712,10 +3743,10 @@
       <c r="H40" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="29" t="s">
+      <c r="I40" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="J40" s="29" t="s">
+      <c r="J40" s="26" t="s">
         <v>283</v>
       </c>
       <c r="K40" s="19" t="s">
@@ -3825,7 +3856,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPàgina &amp;P</oddFooter>

</xml_diff>

<commit_message>
info mails & urls enabled
</commit_message>
<xml_diff>
--- a/src/components/survey_2.xlsx
+++ b/src/components/survey_2.xlsx
@@ -152,7 +152,7 @@
     <t xml:space="preserve">Main Investigation</t>
   </si>
   <si>
-    <t xml:space="preserve">Main results / products</t>
+    <t xml:space="preserve">results</t>
   </si>
   <si>
     <t xml:space="preserve">Mailing address of the supervising organization</t>
@@ -310,7 +310,25 @@
     <t xml:space="preserve">Chemical Engineering School of Sichuan University, Chengdu, Sichuan 610065, China</t>
   </si>
   <si>
-    <t xml:space="preserve">li-yongsheng@scu.edu.cn, lysgxf2005@yahoo.com.cn (Y.-S.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">li-yongsheng@scu.edu.cn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> lysgxf2005@yahoo.com.cn</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Industrial wastewater</t>
@@ -1151,7 +1169,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1219,6 +1237,13 @@
     <font>
       <u val="single"/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1373,7 +1398,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1459,10 +1484,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1474,7 +1503,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1482,19 +1511,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1585,7 +1614,7 @@
       <selection pane="bottomLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="17.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.39"/>
@@ -2094,13 +2123,13 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="46.83"/>
@@ -2360,7 +2389,7 @@
       <c r="L6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="M6" s="15" t="s">
+      <c r="M6" s="21" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2392,7 +2421,7 @@
       <c r="I7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="22" t="s">
         <v>95</v>
       </c>
       <c r="K7" s="18" t="s">
@@ -2433,7 +2462,7 @@
       <c r="I8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="22" t="s">
         <v>104</v>
       </c>
       <c r="K8" s="18" t="s">
@@ -2524,7 +2553,7 @@
       <c r="L10" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="23" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2535,7 +2564,7 @@
       <c r="B11" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="24" t="s">
         <v>122</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -2556,7 +2585,7 @@
       <c r="I11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="22" t="s">
         <v>123</v>
       </c>
       <c r="K11" s="18" t="s">
@@ -2872,7 +2901,7 @@
       <c r="E19" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="25" t="s">
         <v>171</v>
       </c>
       <c r="G19" s="19" t="s">
@@ -2887,7 +2916,7 @@
       <c r="J19" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="25" t="s">
         <v>173</v>
       </c>
       <c r="L19" s="17" t="s">
@@ -2913,7 +2942,7 @@
       <c r="E20" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="25" t="s">
         <v>171</v>
       </c>
       <c r="G20" s="19" t="s">
@@ -3007,7 +3036,7 @@
       <c r="I22" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="J22" s="26" t="s">
         <v>186</v>
       </c>
       <c r="K22" s="18" t="s">
@@ -3048,7 +3077,7 @@
       <c r="I23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="26" t="s">
         <v>190</v>
       </c>
       <c r="K23" s="18" t="s">
@@ -3414,10 +3443,10 @@
       <c r="H32" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="26" t="s">
+      <c r="I32" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="J32" s="27" t="s">
+      <c r="J32" s="28" t="s">
         <v>245</v>
       </c>
       <c r="K32" s="18" t="s">
@@ -3455,10 +3484,10 @@
       <c r="H33" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="26" t="s">
+      <c r="I33" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="27" t="s">
         <v>249</v>
       </c>
       <c r="K33" s="18" t="s">
@@ -3496,10 +3525,10 @@
       <c r="H34" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="27" t="s">
         <v>252</v>
       </c>
       <c r="K34" s="18" t="s">
@@ -3537,10 +3566,10 @@
       <c r="H35" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="26" t="s">
+      <c r="I35" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J35" s="27" t="s">
         <v>254</v>
       </c>
       <c r="K35" s="18" t="s">
@@ -3578,10 +3607,10 @@
       <c r="H36" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I36" s="26" t="s">
+      <c r="I36" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="28" t="s">
+      <c r="J36" s="29" t="s">
         <v>260</v>
       </c>
       <c r="K36" s="18" t="s">
@@ -3590,7 +3619,7 @@
       <c r="L36" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="M36" s="29" t="s">
+      <c r="M36" s="30" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3619,10 +3648,10 @@
       <c r="H37" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="26" t="s">
+      <c r="I37" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="J37" s="26" t="s">
+      <c r="J37" s="27" t="s">
         <v>267</v>
       </c>
       <c r="K37" s="18" t="s">
@@ -3631,7 +3660,7 @@
       <c r="L37" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="M37" s="30" t="s">
+      <c r="M37" s="31" t="s">
         <v>270</v>
       </c>
     </row>
@@ -3660,10 +3689,10 @@
       <c r="H38" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="26" t="s">
+      <c r="I38" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="J38" s="26" t="s">
+      <c r="J38" s="27" t="s">
         <v>272</v>
       </c>
       <c r="K38" s="18" t="s">
@@ -3683,7 +3712,7 @@
       <c r="B39" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="C39" s="23" t="str">
+      <c r="C39" s="24" t="str">
         <f aca="false">D39</f>
         <v>Angers University, GEIHP</v>
       </c>
@@ -3702,10 +3731,10 @@
       <c r="H39" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="I39" s="26" t="s">
+      <c r="I39" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="J39" s="26" t="s">
+      <c r="J39" s="27" t="s">
         <v>278</v>
       </c>
       <c r="K39" s="18" t="s">
@@ -3743,10 +3772,10 @@
       <c r="H40" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="26" t="s">
+      <c r="I40" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="J40" s="26" t="s">
+      <c r="J40" s="27" t="s">
         <v>283</v>
       </c>
       <c r="K40" s="19" t="s">
@@ -3771,88 +3800,89 @@
     <hyperlink ref="F5" r:id="rId8" display="http://www.membraneservices.com/ "/>
     <hyperlink ref="K5" r:id="rId9" display="http://www.membraneservices.com/Recycled_Membranes.html"/>
     <hyperlink ref="K6" r:id="rId10" display="https://www.sciencedirect.com/science/article/pii/S0011916413001756?via%3Dihub"/>
-    <hyperlink ref="F7" r:id="rId11" display="https://eurecat.org/"/>
-    <hyperlink ref="K7" r:id="rId12" display="https://eurecat.org/es/portfolio-items/eflucomp/"/>
-    <hyperlink ref="M7" r:id="rId13" display="xavier.martinez@eurecat.org"/>
-    <hyperlink ref="F8" r:id="rId14" display="http://www.lequia.udg.edu/"/>
-    <hyperlink ref="K8" r:id="rId15" display="http://www.lequia.udg.edu/research/ongoing-projects/item/2621-mem2-0.html"/>
-    <hyperlink ref="M8" r:id="rId16" display=" joaquim.comas@udg.edu "/>
-    <hyperlink ref="K9" r:id="rId17" display="https://doi.org/10.1016/j.desal.2017.12.034"/>
-    <hyperlink ref="M9" r:id="rId18" display="membranas.agua@imdea.org"/>
-    <hyperlink ref="K10" r:id="rId19" display="https://doi.org/10.1016/j.resconrec.2019.104423"/>
-    <hyperlink ref="F11" r:id="rId20" display="http://www.lequia.udg.edu/"/>
-    <hyperlink ref="K11" r:id="rId21" display="http://www.lequia.udg.edu/research/ongoing-projects/item/2621-mem2-0.html"/>
-    <hyperlink ref="M11" r:id="rId22" display=" joaquim.comas@udg.edu "/>
-    <hyperlink ref="F12" r:id="rId23" display="https://en.unifei.edu.br/ "/>
-    <hyperlink ref="K12" r:id="rId24" display="http://journals.sagepub.com/doi/10.1177/0734242X16684383"/>
-    <hyperlink ref="M12" r:id="rId25" display="ecoutinho@unifei.edu.br"/>
-    <hyperlink ref="F13" r:id="rId26" display="http://www.ufrgs.br/ufrgs/inicial"/>
-    <hyperlink ref="K13" r:id="rId27" display="https://www.sciencedirect.com/science/article/pii/S1383586612004108"/>
-    <hyperlink ref="M13" r:id="rId28" display="isabel@enq.ufrgs.br"/>
-    <hyperlink ref="F14" r:id="rId29" display="https://www.medrc.org"/>
-    <hyperlink ref="K14" r:id="rId30" display="https://www.medrc.org/kick-off-meeting-for-membrane-reuse-project/"/>
-    <hyperlink ref="M14" r:id="rId31" display="elkharraz@medrc.org"/>
-    <hyperlink ref="F15" r:id="rId32" display="http://www.ufrgs.br/ufrgs/inicial"/>
-    <hyperlink ref="K15" r:id="rId33" display="https://www.tandfonline.com/doi/abs/10.1080/01496395.2012.745876"/>
-    <hyperlink ref="M15" r:id="rId34" display="alan.ambrosi@gmail.com"/>
-    <hyperlink ref="E16" r:id="rId35" display="University"/>
-    <hyperlink ref="F16" r:id="rId36" display="https://www.ulpgc.es/node "/>
-    <hyperlink ref="K16" r:id="rId37" display="https://www.sciencedirect.com/science/article/pii/S0011916403003849 ; https://www.sciencedirect.com/science/article/pii/S0011916402009773"/>
-    <hyperlink ref="M16" r:id="rId38" display="jveza@dip.ulpgc.es"/>
-    <hyperlink ref="F17" r:id="rId39" display="https://www.unsw.edu.au/"/>
-    <hyperlink ref="K17" r:id="rId40" display="https://doi.org/10.1016/j.memsci.2013.07.015"/>
-    <hyperlink ref="F18" r:id="rId41" display="https://www.unsw.edu.au/"/>
-    <hyperlink ref="K18" r:id="rId42" display="https://doi.org/10.1016/j.desal.2014.10.013"/>
-    <hyperlink ref="F19" r:id="rId43" display="http://www.life-transfomem.eu/publications/"/>
-    <hyperlink ref="K19" r:id="rId44" display="https://www.youtube.com/watch?v=DPp8uYN-iT8&amp;feature=youtu.be"/>
-    <hyperlink ref="M19" r:id="rId45" display="membranas.agua@imdea.org"/>
-    <hyperlink ref="F20" r:id="rId46" display="http://www.life-transfomem.eu/publications/"/>
-    <hyperlink ref="K20" r:id="rId47" display="https://drive.google.com/file/d/1AZxH825pFNvNKMYyNBoTDKOu80dR2DL4/view"/>
-    <hyperlink ref="M20" r:id="rId48" display="membranas.agua@imdea.org"/>
-    <hyperlink ref="K21" r:id="rId49" location="!" display="https://www.sciencedirect.com/science/article/pii/S0959652618314355#!"/>
-    <hyperlink ref="M21" r:id="rId50" display="ecoutinho@desa.ufmg.br"/>
-    <hyperlink ref="K22" r:id="rId51" display="https://nextgenwater.eu/demonstration-cases/costa-brava-region/"/>
-    <hyperlink ref="F24" r:id="rId52" display="https://aquatip.com.au/"/>
-    <hyperlink ref="K24" r:id="rId53" display="https://aquatip.com.au/services/"/>
-    <hyperlink ref="M24" r:id="rId54" display="director@aquatip.com.au"/>
-    <hyperlink ref="F25" r:id="rId55" display="http://www.cerd.dj/"/>
-    <hyperlink ref="K25" r:id="rId56" display="https://www.ncbi.nlm.nih.gov/pubmed/23508163"/>
-    <hyperlink ref="K26" r:id="rId57" display="https://www.sciencedirect.com/science/article/pii/S0043135415304206"/>
-    <hyperlink ref="M26" r:id="rId58" display="m.pype@awmc.uq.edu.au"/>
-    <hyperlink ref="K27" r:id="rId59" display="https://www.sciencedirect.com/science/article/pii/S0011916409013204"/>
-    <hyperlink ref="M27" r:id="rId60" display="maxime.pontie@univ-angers.fr"/>
-    <hyperlink ref="K28" r:id="rId61" display="http://www.zerobrine.eu/pilot-projects/spain/"/>
-    <hyperlink ref="F29" r:id="rId62" location="pagina-ejemplo" display="http://releach.eu/#pagina-ejemplo"/>
-    <hyperlink ref="K29" r:id="rId63" display="http://releach.ctm.com.es/en/the-project/main-project-results"/>
-    <hyperlink ref="M29" r:id="rId64" display="xavier.martinez@eurecat.org"/>
-    <hyperlink ref="F30" r:id="rId65" display="https://www.lut.fi/web/en"/>
-    <hyperlink ref="K30" r:id="rId66" display="https://www.sciencedirect.com/science/article/pii/S0376738818327728"/>
-    <hyperlink ref="M30" r:id="rId67" display="arto.pihlajamaki@lut.fi"/>
-    <hyperlink ref="K31" r:id="rId68" display="https://doi.org/10.1080/09593330.2018.1526218"/>
-    <hyperlink ref="M31" r:id="rId69" display="ecoutinho@desa.ufmg.br"/>
-    <hyperlink ref="F32" r:id="rId70" display="http://www.lequia.udg.edu/"/>
-    <hyperlink ref="K32" r:id="rId71" display="http://www.lequia.udg.edu/research/ongoing-projects/item/2621-mem2-0.html"/>
-    <hyperlink ref="M32" r:id="rId72" display=" joaquim.comas@udg.edu "/>
-    <hyperlink ref="F33" r:id="rId73" display="http://www.agua.imdea.org/infraestructuras-cientificas/plantas-piloto/tecnologia-membranas"/>
-    <hyperlink ref="K33" r:id="rId74" display="http://inremem.simplesite.com/"/>
-    <hyperlink ref="M33" r:id="rId75" display="membranas.agua@imdea.org"/>
-    <hyperlink ref="K34" r:id="rId76" display="https://doi.org/10.1016/j.memsci.2019.117423"/>
-    <hyperlink ref="M34" r:id="rId77" display="membranas.agua@imdea.org"/>
-    <hyperlink ref="K35" r:id="rId78" display="http://dx.doi.org/10.1016/j.scitotenv.2018.07.435"/>
-    <hyperlink ref="M35" r:id="rId79" display="membranas.agua@imdea.org"/>
-    <hyperlink ref="F36" r:id="rId80" display="http://www.remeb-h2020.com/about-us/"/>
-    <hyperlink ref="K36" r:id="rId81" display="http://www.remeb-h2020.com/project-progress/"/>
-    <hyperlink ref="F37" r:id="rId82" display="http://www.memre.de "/>
-    <hyperlink ref="K37" r:id="rId83" display="https://www.dme-gmbh.de/new-founded-company-memre-gmbh/"/>
-    <hyperlink ref="F38" r:id="rId84" display="http://www.univ-nantes.fr/ "/>
-    <hyperlink ref="K38" r:id="rId85" display="https://www.tandfonline.com/doi/abs/10.1080/19443994.2014.943060"/>
-    <hyperlink ref="M38" r:id="rId86" display="maxime.pontie@univ-angers.fr"/>
-    <hyperlink ref="F39" r:id="rId87" display="http://www.univ-angers.fr/fr/recherche/poles-et-unites/pole-sante/geihp.html "/>
-    <hyperlink ref="K39" r:id="rId88" display="https://www.sciencedirect.com/science/article/pii/S0011916417301042 "/>
-    <hyperlink ref="M39" r:id="rId89" display="maxime.pontie@univ-angers.fr"/>
-    <hyperlink ref="F40" r:id="rId90" display="https://www.ucm.es/ "/>
-    <hyperlink ref="K40" r:id="rId91" display="EUROMEMBRANE 2018 CONGRESS: POSTER (N-404) (N-600)"/>
-    <hyperlink ref="M40" r:id="rId92" display="mcgpayo@ucm.es"/>
+    <hyperlink ref="M6" r:id="rId11" display="li-yongsheng@scu.edu.cn"/>
+    <hyperlink ref="F7" r:id="rId12" display="https://eurecat.org/"/>
+    <hyperlink ref="K7" r:id="rId13" display="https://eurecat.org/es/portfolio-items/eflucomp/"/>
+    <hyperlink ref="M7" r:id="rId14" display="xavier.martinez@eurecat.org"/>
+    <hyperlink ref="F8" r:id="rId15" display="http://www.lequia.udg.edu/"/>
+    <hyperlink ref="K8" r:id="rId16" display="http://www.lequia.udg.edu/research/ongoing-projects/item/2621-mem2-0.html"/>
+    <hyperlink ref="M8" r:id="rId17" display=" joaquim.comas@udg.edu "/>
+    <hyperlink ref="K9" r:id="rId18" display="https://doi.org/10.1016/j.desal.2017.12.034"/>
+    <hyperlink ref="M9" r:id="rId19" display="membranas.agua@imdea.org"/>
+    <hyperlink ref="K10" r:id="rId20" display="https://doi.org/10.1016/j.resconrec.2019.104423"/>
+    <hyperlink ref="F11" r:id="rId21" display="http://www.lequia.udg.edu/"/>
+    <hyperlink ref="K11" r:id="rId22" display="http://www.lequia.udg.edu/research/ongoing-projects/item/2621-mem2-0.html"/>
+    <hyperlink ref="M11" r:id="rId23" display=" joaquim.comas@udg.edu "/>
+    <hyperlink ref="F12" r:id="rId24" display="https://en.unifei.edu.br/ "/>
+    <hyperlink ref="K12" r:id="rId25" display="http://journals.sagepub.com/doi/10.1177/0734242X16684383"/>
+    <hyperlink ref="M12" r:id="rId26" display="ecoutinho@unifei.edu.br"/>
+    <hyperlink ref="F13" r:id="rId27" display="http://www.ufrgs.br/ufrgs/inicial"/>
+    <hyperlink ref="K13" r:id="rId28" display="https://www.sciencedirect.com/science/article/pii/S1383586612004108"/>
+    <hyperlink ref="M13" r:id="rId29" display="isabel@enq.ufrgs.br"/>
+    <hyperlink ref="F14" r:id="rId30" display="https://www.medrc.org"/>
+    <hyperlink ref="K14" r:id="rId31" display="https://www.medrc.org/kick-off-meeting-for-membrane-reuse-project/"/>
+    <hyperlink ref="M14" r:id="rId32" display="elkharraz@medrc.org"/>
+    <hyperlink ref="F15" r:id="rId33" display="http://www.ufrgs.br/ufrgs/inicial"/>
+    <hyperlink ref="K15" r:id="rId34" display="https://www.tandfonline.com/doi/abs/10.1080/01496395.2012.745876"/>
+    <hyperlink ref="M15" r:id="rId35" display="alan.ambrosi@gmail.com"/>
+    <hyperlink ref="E16" r:id="rId36" display="University"/>
+    <hyperlink ref="F16" r:id="rId37" display="https://www.ulpgc.es/node "/>
+    <hyperlink ref="K16" r:id="rId38" display="https://www.sciencedirect.com/science/article/pii/S0011916403003849 ; https://www.sciencedirect.com/science/article/pii/S0011916402009773"/>
+    <hyperlink ref="M16" r:id="rId39" display="jveza@dip.ulpgc.es"/>
+    <hyperlink ref="F17" r:id="rId40" display="https://www.unsw.edu.au/"/>
+    <hyperlink ref="K17" r:id="rId41" display="https://doi.org/10.1016/j.memsci.2013.07.015"/>
+    <hyperlink ref="F18" r:id="rId42" display="https://www.unsw.edu.au/"/>
+    <hyperlink ref="K18" r:id="rId43" display="https://doi.org/10.1016/j.desal.2014.10.013"/>
+    <hyperlink ref="F19" r:id="rId44" display="http://www.life-transfomem.eu/publications/"/>
+    <hyperlink ref="K19" r:id="rId45" display="https://www.youtube.com/watch?v=DPp8uYN-iT8&amp;feature=youtu.be"/>
+    <hyperlink ref="M19" r:id="rId46" display="membranas.agua@imdea.org"/>
+    <hyperlink ref="F20" r:id="rId47" display="http://www.life-transfomem.eu/publications/"/>
+    <hyperlink ref="K20" r:id="rId48" display="https://drive.google.com/file/d/1AZxH825pFNvNKMYyNBoTDKOu80dR2DL4/view"/>
+    <hyperlink ref="M20" r:id="rId49" display="membranas.agua@imdea.org"/>
+    <hyperlink ref="K21" r:id="rId50" location="!" display="https://www.sciencedirect.com/science/article/pii/S0959652618314355#!"/>
+    <hyperlink ref="M21" r:id="rId51" display="ecoutinho@desa.ufmg.br"/>
+    <hyperlink ref="K22" r:id="rId52" display="https://nextgenwater.eu/demonstration-cases/costa-brava-region/"/>
+    <hyperlink ref="F24" r:id="rId53" display="https://aquatip.com.au/"/>
+    <hyperlink ref="K24" r:id="rId54" display="https://aquatip.com.au/services/"/>
+    <hyperlink ref="M24" r:id="rId55" display="director@aquatip.com.au"/>
+    <hyperlink ref="F25" r:id="rId56" display="http://www.cerd.dj/"/>
+    <hyperlink ref="K25" r:id="rId57" display="https://www.ncbi.nlm.nih.gov/pubmed/23508163"/>
+    <hyperlink ref="K26" r:id="rId58" display="https://www.sciencedirect.com/science/article/pii/S0043135415304206"/>
+    <hyperlink ref="M26" r:id="rId59" display="m.pype@awmc.uq.edu.au"/>
+    <hyperlink ref="K27" r:id="rId60" display="https://www.sciencedirect.com/science/article/pii/S0011916409013204"/>
+    <hyperlink ref="M27" r:id="rId61" display="maxime.pontie@univ-angers.fr"/>
+    <hyperlink ref="K28" r:id="rId62" display="http://www.zerobrine.eu/pilot-projects/spain/"/>
+    <hyperlink ref="F29" r:id="rId63" location="pagina-ejemplo" display="http://releach.eu/#pagina-ejemplo"/>
+    <hyperlink ref="K29" r:id="rId64" display="http://releach.ctm.com.es/en/the-project/main-project-results"/>
+    <hyperlink ref="M29" r:id="rId65" display="xavier.martinez@eurecat.org"/>
+    <hyperlink ref="F30" r:id="rId66" display="https://www.lut.fi/web/en"/>
+    <hyperlink ref="K30" r:id="rId67" display="https://www.sciencedirect.com/science/article/pii/S0376738818327728"/>
+    <hyperlink ref="M30" r:id="rId68" display="arto.pihlajamaki@lut.fi"/>
+    <hyperlink ref="K31" r:id="rId69" display="https://doi.org/10.1080/09593330.2018.1526218"/>
+    <hyperlink ref="M31" r:id="rId70" display="ecoutinho@desa.ufmg.br"/>
+    <hyperlink ref="F32" r:id="rId71" display="http://www.lequia.udg.edu/"/>
+    <hyperlink ref="K32" r:id="rId72" display="http://www.lequia.udg.edu/research/ongoing-projects/item/2621-mem2-0.html"/>
+    <hyperlink ref="M32" r:id="rId73" display=" joaquim.comas@udg.edu "/>
+    <hyperlink ref="F33" r:id="rId74" display="http://www.agua.imdea.org/infraestructuras-cientificas/plantas-piloto/tecnologia-membranas"/>
+    <hyperlink ref="K33" r:id="rId75" display="http://inremem.simplesite.com/"/>
+    <hyperlink ref="M33" r:id="rId76" display="membranas.agua@imdea.org"/>
+    <hyperlink ref="K34" r:id="rId77" display="https://doi.org/10.1016/j.memsci.2019.117423"/>
+    <hyperlink ref="M34" r:id="rId78" display="membranas.agua@imdea.org"/>
+    <hyperlink ref="K35" r:id="rId79" display="http://dx.doi.org/10.1016/j.scitotenv.2018.07.435"/>
+    <hyperlink ref="M35" r:id="rId80" display="membranas.agua@imdea.org"/>
+    <hyperlink ref="F36" r:id="rId81" display="http://www.remeb-h2020.com/about-us/"/>
+    <hyperlink ref="K36" r:id="rId82" display="http://www.remeb-h2020.com/project-progress/"/>
+    <hyperlink ref="F37" r:id="rId83" display="http://www.memre.de "/>
+    <hyperlink ref="K37" r:id="rId84" display="https://www.dme-gmbh.de/new-founded-company-memre-gmbh/"/>
+    <hyperlink ref="F38" r:id="rId85" display="http://www.univ-nantes.fr/ "/>
+    <hyperlink ref="K38" r:id="rId86" display="https://www.tandfonline.com/doi/abs/10.1080/19443994.2014.943060"/>
+    <hyperlink ref="M38" r:id="rId87" display="maxime.pontie@univ-angers.fr"/>
+    <hyperlink ref="F39" r:id="rId88" display="http://www.univ-angers.fr/fr/recherche/poles-et-unites/pole-sante/geihp.html "/>
+    <hyperlink ref="K39" r:id="rId89" display="https://www.sciencedirect.com/science/article/pii/S0011916417301042 "/>
+    <hyperlink ref="M39" r:id="rId90" display="maxime.pontie@univ-angers.fr"/>
+    <hyperlink ref="F40" r:id="rId91" display="https://www.ucm.es/ "/>
+    <hyperlink ref="K40" r:id="rId92" display="EUROMEMBRANE 2018 CONGRESS: POSTER (N-404) (N-600)"/>
+    <hyperlink ref="M40" r:id="rId93" display="mcgpayo@ucm.es"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>